<commit_message>
Added performance analysis of using the concatenate functionality in the memory tile with 16 AIEs
</commit_message>
<xml_diff>
--- a/gemm/Performance_Results.xlsx
+++ b/gemm/Performance_Results.xlsx
@@ -1,5 +1,5 @@
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1188,7 +1188,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/colors13.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1228,7 +1228,7 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1268,7 +1268,7 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1784,7 +1784,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2302,10 +2302,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3196CDE-7DD8-4B24-B46D-E8AFD451E1FA}">
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E120" sqref="E120"/>
+    <sheetView tabSelected="1" topLeftCell="N29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AJ46" sqref="AJ46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2325,50 +2325,54 @@
     <col min="13" max="13" width="31.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="G1" s="34" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="G1" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="I1" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="P1" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="12"/>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25" t="s">
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="J2" s="23" t="s">
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="K2" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="L2" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="L2" s="23" t="s">
+      <c r="M2" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="N2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>0</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="23"/>
       <c r="B3" s="23" t="s">
         <v>35</v>
@@ -2391,30 +2395,33 @@
       <c r="H3" s="7">
         <v>16</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="7">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="K3" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>73</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="M3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="24">
-        <v>5935.6141090393003</v>
-      </c>
-      <c r="N3" s="14"/>
-      <c r="O3" s="24">
-        <v>5935.6141090393003</v>
-      </c>
+      <c r="N3" s="24">
+        <v>5602.5973796844401</v>
+      </c>
+      <c r="O3" s="14"/>
       <c r="P3" s="24">
-        <v>5935.6141090393003</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+        <v>5602.5973796844401</v>
+      </c>
+      <c r="Q3" s="24">
+        <v>5602.5973796844401</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>33</v>
       </c>
@@ -2437,32 +2444,35 @@
         <v>349.79279041290198</v>
       </c>
       <c r="H4" s="24">
-        <v>88.585853576660099</v>
-      </c>
-      <c r="I4" t="s">
+        <v>88.439083099365206</v>
+      </c>
+      <c r="I4" s="24">
+        <v>108.528447151184</v>
+      </c>
+      <c r="J4" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="K4" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>73</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="M4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="24">
-        <v>1206.1681747436501</v>
-      </c>
-      <c r="N4" s="14"/>
-      <c r="O4" s="24">
-        <v>1206.1681747436501</v>
-      </c>
+      <c r="N4" s="24">
+        <v>1129.1275024414001</v>
+      </c>
+      <c r="O4" s="14"/>
       <c r="P4" s="24">
-        <v>1206.1681747436501</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+        <v>1129.1275024414001</v>
+      </c>
+      <c r="Q4" s="24">
+        <v>1129.1275024414001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>33</v>
       </c>
@@ -2485,32 +2495,35 @@
         <v>88.539719581604004</v>
       </c>
       <c r="H5" s="24">
-        <v>25.6402492523193</v>
-      </c>
-      <c r="I5" t="s">
+        <v>35.051631927490199</v>
+      </c>
+      <c r="I5" s="24">
+        <v>37.345504760742102</v>
+      </c>
+      <c r="J5" t="s">
         <v>4</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>72</v>
       </c>
       <c r="K5" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="M5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="M5" s="24">
-        <v>1529.72507476806</v>
-      </c>
-      <c r="N5" s="14"/>
-      <c r="O5" s="24">
-        <v>1529.72507476806</v>
-      </c>
+      <c r="N5" s="24">
+        <v>1525.2731323242101</v>
+      </c>
+      <c r="O5" s="14"/>
       <c r="P5" s="24">
-        <v>1529.72507476806</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+        <v>1525.2731323242101</v>
+      </c>
+      <c r="Q5" s="24">
+        <v>1525.2731323242101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>33</v>
       </c>
@@ -2533,32 +2546,35 @@
         <v>335.07869243621798</v>
       </c>
       <c r="H6" s="24">
-        <v>80.328464508056598</v>
-      </c>
-      <c r="I6" t="s">
+        <v>91.157484054565401</v>
+      </c>
+      <c r="I6" s="24">
+        <v>88.757967948913503</v>
+      </c>
+      <c r="J6" t="s">
         <v>4</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>72</v>
       </c>
       <c r="K6" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="L6" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="M6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="M6" s="24">
-        <v>684.27348136901799</v>
-      </c>
-      <c r="N6" s="14"/>
-      <c r="O6" s="24">
-        <v>684.27348136901799</v>
-      </c>
+      <c r="N6" s="24">
+        <v>647.73695468902497</v>
+      </c>
+      <c r="O6" s="14"/>
       <c r="P6" s="24">
-        <v>684.27348136901799</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+        <v>647.73695468902497</v>
+      </c>
+      <c r="Q6" s="24">
+        <v>647.73695468902497</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>33</v>
       </c>
@@ -2581,31 +2597,34 @@
         <v>172.97868728637599</v>
       </c>
       <c r="H7" s="24">
-        <v>55.844306945800703</v>
-      </c>
-      <c r="I7" t="s">
+        <v>50.162458419799798</v>
+      </c>
+      <c r="I7" s="24">
+        <v>65.280055999755803</v>
+      </c>
+      <c r="J7" t="s">
         <v>4</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>5</v>
       </c>
       <c r="K7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="L7" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="M7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="M7" s="24">
-        <v>1509.5431804656901</v>
-      </c>
-      <c r="O7" s="24">
-        <v>1509.5431804656901</v>
+      <c r="N7" s="24">
+        <v>1527.2670030593799</v>
       </c>
       <c r="P7" s="24">
-        <v>1509.5431804656901</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+        <v>1527.2670030593799</v>
+      </c>
+      <c r="Q7" s="24">
+        <v>1527.2670030593799</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>33</v>
       </c>
@@ -2628,31 +2647,34 @@
         <v>346.66957855224598</v>
       </c>
       <c r="H8" s="24">
-        <v>88.450193405151296</v>
-      </c>
-      <c r="I8" t="s">
+        <v>91.277098655700598</v>
+      </c>
+      <c r="I8" s="24">
+        <v>77.175593376159597</v>
+      </c>
+      <c r="J8" t="s">
         <v>4</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>5</v>
       </c>
       <c r="K8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="L8" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="M8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="24">
-        <v>644.76513862609795</v>
-      </c>
-      <c r="O8" s="24">
-        <v>644.76513862609795</v>
+      <c r="N8" s="24">
+        <v>727.76646614074696</v>
       </c>
       <c r="P8" s="24">
-        <v>644.76513862609795</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+        <v>727.76646614074696</v>
+      </c>
+      <c r="Q8" s="24">
+        <v>727.76646614074696</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>33</v>
       </c>
@@ -2675,31 +2697,34 @@
         <v>78.713274002075195</v>
       </c>
       <c r="H9" s="24">
-        <v>39.356470108032198</v>
-      </c>
-      <c r="I9" t="s">
+        <v>29.814243316650298</v>
+      </c>
+      <c r="I9" s="24">
+        <v>31.673622131347599</v>
+      </c>
+      <c r="J9" t="s">
         <v>4</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="K9" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>74</v>
       </c>
-      <c r="L9" s="7" t="s">
+      <c r="M9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="M9" s="24">
-        <v>16.215562820434499</v>
-      </c>
-      <c r="O9" s="24">
-        <v>16.215562820434499</v>
+      <c r="N9" s="24">
+        <v>10.190629959106399</v>
       </c>
       <c r="P9" s="24">
-        <v>16.215562820434499</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+        <v>10.190629959106399</v>
+      </c>
+      <c r="Q9" s="24">
+        <v>10.190629959106399</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>33</v>
       </c>
@@ -2722,31 +2747,34 @@
         <v>339.62914943695</v>
       </c>
       <c r="H10" s="24">
-        <v>77.983379364013601</v>
-      </c>
-      <c r="I10" t="s">
+        <v>82.832837104797306</v>
+      </c>
+      <c r="I10" s="24">
+        <v>70.231199264526296</v>
+      </c>
+      <c r="J10" t="s">
         <v>4</v>
       </c>
-      <c r="J10" s="12" t="s">
+      <c r="K10" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>74</v>
       </c>
-      <c r="L10" s="7" t="s">
+      <c r="M10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="M10" s="24">
-        <v>38.001298904418903</v>
-      </c>
-      <c r="O10" s="24">
-        <v>38.001298904418903</v>
+      <c r="N10" s="24">
+        <v>36.996316909790004</v>
       </c>
       <c r="P10" s="24">
-        <v>38.001298904418903</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+        <v>36.996316909790004</v>
+      </c>
+      <c r="Q10" s="24">
+        <v>36.996316909790004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>33</v>
       </c>
@@ -2769,31 +2797,37 @@
         <v>187.67244815826399</v>
       </c>
       <c r="H11" s="24">
-        <v>49.073696136474602</v>
-      </c>
-      <c r="I11" t="s">
+        <v>52.835321426391602</v>
+      </c>
+      <c r="I11" s="24">
+        <v>58.136677742004302</v>
+      </c>
+      <c r="J11" t="s">
         <v>4</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>75</v>
       </c>
       <c r="K11" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="L11" s="7" t="s">
+      <c r="L11" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="M11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="M11" s="24">
-        <v>4772.7956771850504</v>
-      </c>
-      <c r="O11" s="24">
-        <v>4772.7956771850504</v>
+      <c r="N11" s="24">
+        <v>4716.1022663116401</v>
       </c>
       <c r="P11" s="24">
-        <v>4772.7956771850504</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+        <v>4716.1022663116401</v>
+      </c>
+      <c r="Q11" s="24">
+        <v>4716.1022663116401</v>
+      </c>
+      <c r="R11" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>33</v>
       </c>
@@ -2816,31 +2850,34 @@
         <v>327.440118789672</v>
       </c>
       <c r="H12" s="24">
-        <v>88.159799575805593</v>
-      </c>
-      <c r="I12" t="s">
+        <v>90.101504325866699</v>
+      </c>
+      <c r="I12" s="24">
+        <v>81.354117393493596</v>
+      </c>
+      <c r="J12" t="s">
         <v>4</v>
-      </c>
-      <c r="J12" s="12" t="s">
-        <v>75</v>
       </c>
       <c r="K12" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="L12" s="7" t="s">
+      <c r="L12" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="M12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="M12" s="24">
-        <v>1740.28944969177</v>
-      </c>
-      <c r="O12" s="24">
-        <v>1740.28944969177</v>
+      <c r="N12" s="24">
+        <v>1722.4748134613001</v>
       </c>
       <c r="P12" s="24">
-        <v>1740.28944969177</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+        <v>1722.4748134613001</v>
+      </c>
+      <c r="Q12" s="24">
+        <v>1722.4748134613001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>33</v>
       </c>
@@ -2863,10 +2900,13 @@
         <v>179.23693656921299</v>
       </c>
       <c r="H13" s="24">
-        <v>58.935165405273402</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+        <v>50.256061553955</v>
+      </c>
+      <c r="I13" s="24">
+        <v>64.868521690368596</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>33</v>
       </c>
@@ -2889,10 +2929,13 @@
         <v>2545.9532976150499</v>
       </c>
       <c r="H14" s="24">
-        <v>630.84030151367097</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+        <v>627.75597572326603</v>
+      </c>
+      <c r="I14" s="24">
+        <v>416.438913345336</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>33</v>
       </c>
@@ -2915,10 +2958,13 @@
         <v>132.71672725677399</v>
       </c>
       <c r="H15" s="24">
-        <v>59.303998947143498</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+        <v>75.055694580078097</v>
+      </c>
+      <c r="I15" s="24">
+        <v>77.454710006713796</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
         <v>33</v>
       </c>
@@ -2941,10 +2987,13 @@
         <v>636.26639842987004</v>
       </c>
       <c r="H16" s="24">
-        <v>181.99062347412101</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+        <v>181.57274723052899</v>
+      </c>
+      <c r="I16" s="24">
+        <v>119.46225166320799</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>33</v>
       </c>
@@ -2967,10 +3016,13 @@
         <v>353.99408340454102</v>
       </c>
       <c r="H17" s="24">
-        <v>99.988222122192298</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+        <v>125.227642059326</v>
+      </c>
+      <c r="I17" s="24">
+        <v>130.24218082427899</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>33</v>
       </c>
@@ -2993,10 +3045,13 @@
         <v>2577.0546197891199</v>
       </c>
       <c r="H18" s="24">
-        <v>672.26934432983398</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+        <v>655.80103397369305</v>
+      </c>
+      <c r="I18" s="24">
+        <v>579.57146167755104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>33</v>
       </c>
@@ -3019,10 +3074,13 @@
         <v>109.989714622497</v>
       </c>
       <c r="H19" s="24">
-        <v>57.830572128295898</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+        <v>60.235357284545898</v>
+      </c>
+      <c r="I19" s="24">
+        <v>61.998915672302203</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>33</v>
       </c>
@@ -3045,10 +3103,13 @@
         <v>721.73857688903797</v>
       </c>
       <c r="H20" s="24">
-        <v>178.51066589355401</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+        <v>184.496927261352</v>
+      </c>
+      <c r="I20" s="24">
+        <v>185.083484649658</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
         <v>33</v>
       </c>
@@ -3071,10 +3132,13 @@
         <v>367.87891387939402</v>
       </c>
       <c r="H21" s="24">
-        <v>101.938724517822</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+        <v>114.971089363098</v>
+      </c>
+      <c r="I21" s="24">
+        <v>113.276624679565</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="12"/>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
@@ -3083,14 +3147,14 @@
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="F2:H2"/>
     <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3099,10 +3163,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22A96D9F-BFBD-46AC-A0B7-AB81248FE666}">
-  <dimension ref="A1:H93"/>
+  <dimension ref="A1:H124"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="E92" sqref="E92:E93"/>
+    <sheetView topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="H80" activeCellId="3" sqref="H70 H72 H78 H80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4423,6 +4487,11 @@
         <v>789.66953754425003</v>
       </c>
     </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>80</v>
+      </c>
+    </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>0</v>
@@ -4469,10 +4538,10 @@
         <v>42</v>
       </c>
       <c r="G65" s="24">
-        <v>77.636003494262695</v>
+        <v>81.046652793884206</v>
       </c>
       <c r="H65" s="24">
-        <v>88.585853576660099</v>
+        <v>88.439083099365206</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
@@ -4495,10 +4564,10 @@
         <v>45</v>
       </c>
       <c r="G66" s="24">
-        <v>594.97451782226506</v>
+        <v>591.03634357452302</v>
       </c>
       <c r="H66" s="24">
-        <v>630.84030151367097</v>
+        <v>627.75597572326603</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
@@ -4521,10 +4590,10 @@
         <v>47</v>
       </c>
       <c r="G67" s="24">
-        <v>22.269248962402301</v>
+        <v>32.0436239242553</v>
       </c>
       <c r="H67" s="24">
-        <v>25.6402492523193</v>
+        <v>35.051631927490199</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
@@ -4547,10 +4616,10 @@
         <v>48</v>
       </c>
       <c r="G68" s="24">
-        <v>52.283287048339801</v>
+        <v>66.1764621734619</v>
       </c>
       <c r="H68" s="24">
-        <v>59.303998947143498</v>
+        <v>75.055694580078097</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
@@ -4573,10 +4642,10 @@
         <v>42</v>
       </c>
       <c r="G69" s="24">
-        <v>72.0889568328857</v>
+        <v>79.364037513732896</v>
       </c>
       <c r="H69" s="24">
-        <v>88.450193405151296</v>
+        <v>91.277098655700598</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
@@ -4599,10 +4668,10 @@
         <v>45</v>
       </c>
       <c r="G70" s="24">
-        <v>626.68013572692803</v>
+        <v>617.08080768585205</v>
       </c>
       <c r="H70" s="24">
-        <v>672.26934432983398</v>
+        <v>655.80103397369305</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
@@ -4625,10 +4694,10 @@
         <v>47</v>
       </c>
       <c r="G71" s="24">
-        <v>36.343336105346602</v>
+        <v>25.6085157394409</v>
       </c>
       <c r="H71" s="24">
-        <v>39.356470108032198</v>
+        <v>29.814243316650298</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
@@ -4651,10 +4720,10 @@
         <v>48</v>
       </c>
       <c r="G72" s="24">
-        <v>49.472570419311502</v>
+        <v>49.512720108032198</v>
       </c>
       <c r="H72" s="24">
-        <v>57.830572128295898</v>
+        <v>60.235357284545898</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
@@ -4677,10 +4746,10 @@
         <v>49</v>
       </c>
       <c r="G73" s="24">
-        <v>71.796178817748995</v>
+        <v>84.143042564392005</v>
       </c>
       <c r="H73" s="24">
-        <v>80.328464508056598</v>
+        <v>91.157484054565401</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
@@ -4703,10 +4772,10 @@
         <v>50</v>
       </c>
       <c r="G74" s="24">
-        <v>167.33765602111799</v>
+        <v>168.06826591491699</v>
       </c>
       <c r="H74" s="24">
-        <v>181.99062347412101</v>
+        <v>181.57274723052899</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
@@ -4729,10 +4798,10 @@
         <v>51</v>
       </c>
       <c r="G75" s="24">
-        <v>51.807403564453097</v>
+        <v>45.983314514160099</v>
       </c>
       <c r="H75" s="24">
-        <v>55.844306945800703</v>
+        <v>50.162458419799798</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
@@ -4755,10 +4824,10 @@
         <v>52</v>
       </c>
       <c r="G76" s="24">
-        <v>92.985153198242102</v>
+        <v>116.271901130676</v>
       </c>
       <c r="H76" s="24">
-        <v>99.988222122192298</v>
+        <v>125.227642059326</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
@@ -4781,10 +4850,10 @@
         <v>49</v>
       </c>
       <c r="G77" s="24">
-        <v>68.115711212158203</v>
+        <v>76.623225212097097</v>
       </c>
       <c r="H77" s="24">
-        <v>77.983379364013601</v>
+        <v>82.832837104797306</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
@@ -4807,10 +4876,10 @@
         <v>50</v>
       </c>
       <c r="G78" s="24">
-        <v>172.50657081604001</v>
+        <v>172.020030021667</v>
       </c>
       <c r="H78" s="24">
-        <v>178.51066589355401</v>
+        <v>184.496927261352</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
@@ -4833,10 +4902,10 @@
         <v>51</v>
       </c>
       <c r="G79" s="24">
-        <v>46.982288360595703</v>
+        <v>47.1878051757812</v>
       </c>
       <c r="H79" s="24">
-        <v>49.073696136474602</v>
+        <v>52.835321426391602</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
@@ -4859,10 +4928,10 @@
         <v>52</v>
       </c>
       <c r="G80" s="24">
-        <v>87.054252624511705</v>
+        <v>104.697108268737</v>
       </c>
       <c r="H80" s="24">
-        <v>101.938724517822</v>
+        <v>114.971089363098</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.3">
@@ -4885,10 +4954,10 @@
         <v>49</v>
       </c>
       <c r="G81" s="24">
-        <v>81.380367279052706</v>
+        <v>81.493687629699707</v>
       </c>
       <c r="H81" s="24">
-        <v>88.159799575805593</v>
+        <v>90.101504325866699</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.3">
@@ -4911,10 +4980,10 @@
         <v>51</v>
       </c>
       <c r="G82" s="24">
-        <v>52.429676055908203</v>
+        <v>44.741034507751401</v>
       </c>
       <c r="H82" s="24">
-        <v>58.935165405273402</v>
+        <v>50.256061553955</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
@@ -4945,7 +5014,7 @@
         <v>41</v>
       </c>
       <c r="E84" s="24">
-        <v>5935.6141090393003</v>
+        <v>5603.4663915634101</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.3">
@@ -4959,7 +5028,7 @@
         <v>41</v>
       </c>
       <c r="E85" s="24">
-        <v>16.215562820434499</v>
+        <v>8.5654735565185494</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
@@ -4973,7 +5042,7 @@
         <v>46</v>
       </c>
       <c r="E86" s="24">
-        <v>1206.1681747436501</v>
+        <v>1138.49854469299</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.3">
@@ -4987,7 +5056,7 @@
         <v>46</v>
       </c>
       <c r="E87" s="24">
-        <v>38.001298904418903</v>
+        <v>37.660574913024902</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.3">
@@ -5001,7 +5070,7 @@
         <v>41</v>
       </c>
       <c r="E88" s="24">
-        <v>1529.72507476806</v>
+        <v>1509.2229604721001</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
@@ -5015,7 +5084,7 @@
         <v>41</v>
       </c>
       <c r="E89" s="24">
-        <v>4772.7956771850504</v>
+        <v>4661.41269207</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
@@ -5029,7 +5098,7 @@
         <v>46</v>
       </c>
       <c r="E90" s="24">
-        <v>684.27348136901799</v>
+        <v>638.90047073364201</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
@@ -5043,7 +5112,7 @@
         <v>46</v>
       </c>
       <c r="E91" s="24">
-        <v>1740.28944969177</v>
+        <v>1722.53415584564</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
@@ -5057,7 +5126,7 @@
         <v>41</v>
       </c>
       <c r="E92" s="24">
-        <v>1509.5431804656901</v>
+        <v>1516.88463687896</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.3">
@@ -5071,7 +5140,663 @@
         <v>46</v>
       </c>
       <c r="E93" s="24">
-        <v>644.76513862609795</v>
+        <v>663.06173801422096</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>0</v>
+      </c>
+      <c r="B95" t="s">
+        <v>35</v>
+      </c>
+      <c r="C95" t="s">
+        <v>36</v>
+      </c>
+      <c r="D95" t="s">
+        <v>8</v>
+      </c>
+      <c r="E95" t="s">
+        <v>2</v>
+      </c>
+      <c r="F95" t="s">
+        <v>3</v>
+      </c>
+      <c r="G95" t="s">
+        <v>37</v>
+      </c>
+      <c r="H95" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>16</v>
+      </c>
+      <c r="B96" t="s">
+        <v>39</v>
+      </c>
+      <c r="C96" t="s">
+        <v>40</v>
+      </c>
+      <c r="D96" t="s">
+        <v>41</v>
+      </c>
+      <c r="E96" t="s">
+        <v>63</v>
+      </c>
+      <c r="F96" t="s">
+        <v>42</v>
+      </c>
+      <c r="G96" s="24">
+        <v>97.852206230163503</v>
+      </c>
+      <c r="H96" s="24">
+        <v>108.528447151184</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>16</v>
+      </c>
+      <c r="B97" t="s">
+        <v>43</v>
+      </c>
+      <c r="C97" t="s">
+        <v>44</v>
+      </c>
+      <c r="D97" t="s">
+        <v>41</v>
+      </c>
+      <c r="E97" t="s">
+        <v>64</v>
+      </c>
+      <c r="F97" t="s">
+        <v>45</v>
+      </c>
+      <c r="G97" s="24">
+        <v>380.50017356872502</v>
+      </c>
+      <c r="H97" s="24">
+        <v>416.438913345336</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>16</v>
+      </c>
+      <c r="B98" t="s">
+        <v>39</v>
+      </c>
+      <c r="C98" t="s">
+        <v>40</v>
+      </c>
+      <c r="D98" t="s">
+        <v>46</v>
+      </c>
+      <c r="E98" t="s">
+        <v>65</v>
+      </c>
+      <c r="F98" t="s">
+        <v>47</v>
+      </c>
+      <c r="G98" s="24">
+        <v>33.360147476196197</v>
+      </c>
+      <c r="H98" s="24">
+        <v>37.345504760742102</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>16</v>
+      </c>
+      <c r="B99" t="s">
+        <v>43</v>
+      </c>
+      <c r="C99" t="s">
+        <v>44</v>
+      </c>
+      <c r="D99" t="s">
+        <v>46</v>
+      </c>
+      <c r="E99" t="s">
+        <v>66</v>
+      </c>
+      <c r="F99" t="s">
+        <v>48</v>
+      </c>
+      <c r="G99" s="24">
+        <v>66.099548339843693</v>
+      </c>
+      <c r="H99" s="24">
+        <v>77.454710006713796</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>16</v>
+      </c>
+      <c r="B100" t="s">
+        <v>39</v>
+      </c>
+      <c r="C100" t="s">
+        <v>39</v>
+      </c>
+      <c r="D100" t="s">
+        <v>41</v>
+      </c>
+      <c r="E100" t="s">
+        <v>63</v>
+      </c>
+      <c r="F100" t="s">
+        <v>42</v>
+      </c>
+      <c r="G100" s="24">
+        <v>72.629475593566895</v>
+      </c>
+      <c r="H100" s="24">
+        <v>77.175593376159597</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>16</v>
+      </c>
+      <c r="B101" t="s">
+        <v>43</v>
+      </c>
+      <c r="C101" t="s">
+        <v>43</v>
+      </c>
+      <c r="D101" t="s">
+        <v>41</v>
+      </c>
+      <c r="E101" t="s">
+        <v>64</v>
+      </c>
+      <c r="F101" t="s">
+        <v>45</v>
+      </c>
+      <c r="G101" s="24">
+        <v>543.20113658904995</v>
+      </c>
+      <c r="H101" s="24">
+        <v>579.57146167755104</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>16</v>
+      </c>
+      <c r="B102" t="s">
+        <v>39</v>
+      </c>
+      <c r="C102" t="s">
+        <v>39</v>
+      </c>
+      <c r="D102" t="s">
+        <v>46</v>
+      </c>
+      <c r="E102" t="s">
+        <v>65</v>
+      </c>
+      <c r="F102" t="s">
+        <v>47</v>
+      </c>
+      <c r="G102" s="24">
+        <v>26.168966293334901</v>
+      </c>
+      <c r="H102" s="24">
+        <v>31.673622131347599</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>16</v>
+      </c>
+      <c r="B103" t="s">
+        <v>43</v>
+      </c>
+      <c r="C103" t="s">
+        <v>43</v>
+      </c>
+      <c r="D103" t="s">
+        <v>46</v>
+      </c>
+      <c r="E103" t="s">
+        <v>66</v>
+      </c>
+      <c r="F103" t="s">
+        <v>48</v>
+      </c>
+      <c r="G103" s="24">
+        <v>52.126693725585902</v>
+      </c>
+      <c r="H103" s="24">
+        <v>61.998915672302203</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>16</v>
+      </c>
+      <c r="B104" t="s">
+        <v>39</v>
+      </c>
+      <c r="C104" t="s">
+        <v>40</v>
+      </c>
+      <c r="D104" t="s">
+        <v>41</v>
+      </c>
+      <c r="E104" t="s">
+        <v>67</v>
+      </c>
+      <c r="F104" t="s">
+        <v>49</v>
+      </c>
+      <c r="G104" s="24">
+        <v>83.588337898254395</v>
+      </c>
+      <c r="H104" s="24">
+        <v>88.757967948913503</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>16</v>
+      </c>
+      <c r="B105" t="s">
+        <v>43</v>
+      </c>
+      <c r="C105" t="s">
+        <v>44</v>
+      </c>
+      <c r="D105" t="s">
+        <v>41</v>
+      </c>
+      <c r="E105" t="s">
+        <v>68</v>
+      </c>
+      <c r="F105" t="s">
+        <v>50</v>
+      </c>
+      <c r="G105" s="24">
+        <v>112.718892097473</v>
+      </c>
+      <c r="H105" s="24">
+        <v>119.46225166320799</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>16</v>
+      </c>
+      <c r="B106" t="s">
+        <v>39</v>
+      </c>
+      <c r="C106" t="s">
+        <v>40</v>
+      </c>
+      <c r="D106" t="s">
+        <v>46</v>
+      </c>
+      <c r="E106" t="s">
+        <v>69</v>
+      </c>
+      <c r="F106" t="s">
+        <v>51</v>
+      </c>
+      <c r="G106" s="24">
+        <v>59.332156181335399</v>
+      </c>
+      <c r="H106" s="24">
+        <v>65.280055999755803</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>16</v>
+      </c>
+      <c r="B107" t="s">
+        <v>43</v>
+      </c>
+      <c r="C107" t="s">
+        <v>44</v>
+      </c>
+      <c r="D107" t="s">
+        <v>46</v>
+      </c>
+      <c r="E107" t="s">
+        <v>70</v>
+      </c>
+      <c r="F107" t="s">
+        <v>52</v>
+      </c>
+      <c r="G107" s="24">
+        <v>117.02435016632</v>
+      </c>
+      <c r="H107" s="24">
+        <v>130.24218082427899</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>16</v>
+      </c>
+      <c r="B108" t="s">
+        <v>39</v>
+      </c>
+      <c r="C108" t="s">
+        <v>39</v>
+      </c>
+      <c r="D108" t="s">
+        <v>41</v>
+      </c>
+      <c r="E108" t="s">
+        <v>67</v>
+      </c>
+      <c r="F108" t="s">
+        <v>49</v>
+      </c>
+      <c r="G108" s="24">
+        <v>66.201591491699205</v>
+      </c>
+      <c r="H108" s="24">
+        <v>70.231199264526296</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>16</v>
+      </c>
+      <c r="B109" t="s">
+        <v>43</v>
+      </c>
+      <c r="C109" t="s">
+        <v>43</v>
+      </c>
+      <c r="D109" t="s">
+        <v>41</v>
+      </c>
+      <c r="E109" t="s">
+        <v>68</v>
+      </c>
+      <c r="F109" t="s">
+        <v>50</v>
+      </c>
+      <c r="G109" s="24">
+        <v>168.291282653808</v>
+      </c>
+      <c r="H109" s="24">
+        <v>185.083484649658</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>16</v>
+      </c>
+      <c r="B110" t="s">
+        <v>39</v>
+      </c>
+      <c r="C110" t="s">
+        <v>39</v>
+      </c>
+      <c r="D110" t="s">
+        <v>46</v>
+      </c>
+      <c r="E110" t="s">
+        <v>69</v>
+      </c>
+      <c r="F110" t="s">
+        <v>51</v>
+      </c>
+      <c r="G110" s="24">
+        <v>51.389670372009199</v>
+      </c>
+      <c r="H110" s="24">
+        <v>58.136677742004302</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>16</v>
+      </c>
+      <c r="B111" t="s">
+        <v>43</v>
+      </c>
+      <c r="C111" t="s">
+        <v>43</v>
+      </c>
+      <c r="D111" t="s">
+        <v>46</v>
+      </c>
+      <c r="E111" t="s">
+        <v>70</v>
+      </c>
+      <c r="F111" t="s">
+        <v>52</v>
+      </c>
+      <c r="G111" s="24">
+        <v>101.811051368713</v>
+      </c>
+      <c r="H111" s="24">
+        <v>113.276624679565</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>16</v>
+      </c>
+      <c r="B112" t="s">
+        <v>53</v>
+      </c>
+      <c r="C112" t="s">
+        <v>53</v>
+      </c>
+      <c r="D112" t="s">
+        <v>41</v>
+      </c>
+      <c r="E112" t="s">
+        <v>67</v>
+      </c>
+      <c r="F112" t="s">
+        <v>49</v>
+      </c>
+      <c r="G112" s="24">
+        <v>76.450443267822195</v>
+      </c>
+      <c r="H112" s="24">
+        <v>81.354117393493596</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>16</v>
+      </c>
+      <c r="B113" t="s">
+        <v>53</v>
+      </c>
+      <c r="C113" t="s">
+        <v>53</v>
+      </c>
+      <c r="D113" t="s">
+        <v>46</v>
+      </c>
+      <c r="E113" t="s">
+        <v>69</v>
+      </c>
+      <c r="F113" t="s">
+        <v>51</v>
+      </c>
+      <c r="G113" s="24">
+        <v>57.201266288757303</v>
+      </c>
+      <c r="H113" s="24">
+        <v>64.868521690368596</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>4</v>
+      </c>
+      <c r="B114" t="s">
+        <v>35</v>
+      </c>
+      <c r="C114" t="s">
+        <v>36</v>
+      </c>
+      <c r="D114" t="s">
+        <v>8</v>
+      </c>
+      <c r="E114" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B115" t="s">
+        <v>39</v>
+      </c>
+      <c r="C115" t="s">
+        <v>40</v>
+      </c>
+      <c r="D115" t="s">
+        <v>41</v>
+      </c>
+      <c r="E115" s="24">
+        <v>5600.4622936248697</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B116" t="s">
+        <v>55</v>
+      </c>
+      <c r="C116" t="s">
+        <v>44</v>
+      </c>
+      <c r="D116" t="s">
+        <v>41</v>
+      </c>
+      <c r="E116" s="24">
+        <v>13.1986379623413</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B117" t="s">
+        <v>39</v>
+      </c>
+      <c r="C117" t="s">
+        <v>40</v>
+      </c>
+      <c r="D117" t="s">
+        <v>46</v>
+      </c>
+      <c r="E117" s="24">
+        <v>1130.4092168807899</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B118" t="s">
+        <v>55</v>
+      </c>
+      <c r="C118" t="s">
+        <v>44</v>
+      </c>
+      <c r="D118" t="s">
+        <v>46</v>
+      </c>
+      <c r="E118" s="24">
+        <v>37.013983726501401</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B119" t="s">
+        <v>39</v>
+      </c>
+      <c r="C119" t="s">
+        <v>39</v>
+      </c>
+      <c r="D119" t="s">
+        <v>41</v>
+      </c>
+      <c r="E119" s="24">
+        <v>1512.9376649856499</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B120" t="s">
+        <v>55</v>
+      </c>
+      <c r="C120" t="s">
+        <v>55</v>
+      </c>
+      <c r="D120" t="s">
+        <v>41</v>
+      </c>
+      <c r="E120" s="24">
+        <v>4677.09131240844</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B121" t="s">
+        <v>39</v>
+      </c>
+      <c r="C121" t="s">
+        <v>39</v>
+      </c>
+      <c r="D121" t="s">
+        <v>46</v>
+      </c>
+      <c r="E121" s="24">
+        <v>656.31177425384499</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B122" t="s">
+        <v>55</v>
+      </c>
+      <c r="C122" t="s">
+        <v>55</v>
+      </c>
+      <c r="D122" t="s">
+        <v>46</v>
+      </c>
+      <c r="E122" s="24">
+        <v>1716.4659023284901</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B123" t="s">
+        <v>53</v>
+      </c>
+      <c r="C123" t="s">
+        <v>53</v>
+      </c>
+      <c r="D123" t="s">
+        <v>41</v>
+      </c>
+      <c r="E123" s="24">
+        <v>1492.0829534530601</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B124" t="s">
+        <v>53</v>
+      </c>
+      <c r="C124" t="s">
+        <v>53</v>
+      </c>
+      <c r="D124" t="s">
+        <v>46</v>
+      </c>
+      <c r="E124" s="24">
+        <v>646.25608921051003</v>
       </c>
     </row>
   </sheetData>
@@ -5084,8 +5809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D402E31-C37D-4793-A991-19CCD6BD68C2}">
   <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="D7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5101,18 +5826,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
       <c r="I1" t="s">
         <v>13</v>
       </c>
@@ -5150,13 +5875,13 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="28">
+      <c r="A3" s="29">
         <v>1</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="30" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="21" t="s">
@@ -5176,11 +5901,11 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="28"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="30"/>
+      <c r="C4" s="31"/>
       <c r="D4" s="22" t="s">
         <v>32</v>
       </c>
@@ -5198,11 +5923,11 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="28"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="26" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="22" t="s">
@@ -5222,11 +5947,11 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="28"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="31"/>
+      <c r="C6" s="32"/>
       <c r="D6" s="13" t="s">
         <v>27</v>
       </c>
@@ -5244,13 +5969,13 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="28">
+      <c r="A7" s="29">
         <v>4</v>
       </c>
       <c r="B7" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="30" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="21" t="s">
@@ -5270,11 +5995,11 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="28"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="30"/>
+      <c r="C8" s="31"/>
       <c r="D8" s="22" t="s">
         <v>29</v>
       </c>
@@ -5292,11 +6017,11 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="28"/>
+      <c r="A9" s="29"/>
       <c r="B9" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="33" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="22" t="s">
@@ -5316,11 +6041,11 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="28"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="33"/>
+      <c r="C10" s="34"/>
       <c r="D10" s="13" t="s">
         <v>31</v>
       </c>
@@ -5338,13 +6063,13 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="28">
+      <c r="A11" s="29">
         <v>16</v>
       </c>
       <c r="B11" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="30" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="21" t="s">
@@ -5364,11 +6089,11 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="28"/>
+      <c r="A12" s="29"/>
       <c r="B12" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="30"/>
+      <c r="C12" s="31"/>
       <c r="D12" s="22" t="s">
         <v>21</v>
       </c>
@@ -5386,11 +6111,11 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="28"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="33" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="22" t="s">
@@ -5410,11 +6135,11 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="28"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="33"/>
+      <c r="C14" s="34"/>
       <c r="D14" s="13" t="s">
         <v>23</v>
       </c>
@@ -5557,10 +6282,10 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="12"/>
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="27"/>
+      <c r="C23" s="28"/>
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
     </row>

</xml_diff>